<commit_message>
The Hole Code been Abstracted into classes :)
</commit_message>
<xml_diff>
--- a/Task 5/code/NT-33A_4.xlsx
+++ b/Task 5/code/NT-33A_4.xlsx
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>

</xml_diff>